<commit_message>
fixed instructor view, need to handle error
</commit_message>
<xml_diff>
--- a/sampledata/Sample GA submission 2.xlsx
+++ b/sampledata/Sample GA submission 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24617"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\OneDrive\Desktop\graph-reporting-tool\sampledata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D223244B-6202-4438-8B8D-25F0B3F59E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5389A6A6-26B7-4674-9614-C37F2E211596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{20377A6A-3C5C-4288-B408-0C689792B574}"/>
+    <workbookView xWindow="4665" yWindow="5370" windowWidth="28800" windowHeight="15435" xr2:uid="{20377A6A-3C5C-4288-B408-0C689792B574}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,21 +45,6 @@
     <t>First Name</t>
   </si>
   <si>
-    <t>GA 7.3</t>
-  </si>
-  <si>
-    <t>GA 7.5</t>
-  </si>
-  <si>
-    <t>GA 8.4</t>
-  </si>
-  <si>
-    <t>GA 8.6</t>
-  </si>
-  <si>
-    <t>GA 8.8</t>
-  </si>
-  <si>
     <t>JXBU</t>
   </si>
   <si>
@@ -196,13 +181,28 @@
   </si>
   <si>
     <t>SVSR</t>
+  </si>
+  <si>
+    <t>GA 3.1</t>
+  </si>
+  <si>
+    <t>GA 8.1</t>
+  </si>
+  <si>
+    <t>GA 10.3</t>
+  </si>
+  <si>
+    <t>GA 5.2</t>
+  </si>
+  <si>
+    <t>GA 4.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,12 +567,12 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,30 +583,30 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>78239783</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
         <v>3</v>
@@ -624,15 +624,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>53020119</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -650,15 +650,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>54363858</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -676,15 +676,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>12124360</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>4</v>
@@ -702,15 +702,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>97266735</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2">
         <v>3</v>
@@ -728,15 +728,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>11771866</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2">
         <v>2</v>
@@ -754,15 +754,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>24860491</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2">
         <v>3</v>
@@ -780,15 +780,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>72561101</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2">
         <v>4</v>
@@ -806,15 +806,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>83030173</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2">
         <v>3</v>
@@ -832,15 +832,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>71965117</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
@@ -858,15 +858,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>68568782</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
@@ -884,15 +884,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>65692119</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -910,15 +910,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>30631707</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
@@ -936,15 +936,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>97140965</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2">
         <v>4</v>
@@ -962,15 +962,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>28224691</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -988,15 +988,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>41827291</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -1014,15 +1014,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>22981439</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2">
         <v>4</v>
@@ -1040,15 +1040,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>46465284</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2">
         <v>3</v>
@@ -1066,15 +1066,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>36067426</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2">
         <v>3</v>
@@ -1092,15 +1092,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>88057687</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2">
         <v>4</v>
@@ -1118,15 +1118,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>36194465</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2">
         <v>2</v>
@@ -1144,15 +1144,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44088435</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D23" s="2">
         <v>4</v>
@@ -1170,15 +1170,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>10480359</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D24" s="2">
         <v>4</v>

</xml_diff>